<commit_message>
Connect to LSE and loop over multiple companies
</commit_message>
<xml_diff>
--- a/test_data.xlsx
+++ b/test_data.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Harry\Python\Financial_data_scraper\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F3AE822-DBCD-44BB-A87A-0A3A16CFE062}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{207A9435-99DB-4D19-B949-3E83DEDA59AE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{615F4171-48AE-47AC-B24C-1787BFE18D48}"/>
   </bookViews>
@@ -47,25 +47,25 @@
     <t>Water Intelligence</t>
   </si>
   <si>
+    <t>https://www.londonstockexchange.com/stock/AFS/amiad-water-systems-ltd/fundamentals</t>
+  </si>
+  <si>
+    <t>https://www.londonstockexchange.com/stock/WATR/water-intelligence-plc/fundamentals</t>
+  </si>
+  <si>
     <t>RPS Group</t>
   </si>
   <si>
+    <t>https://www.londonstockexchange.com/stock/RPS/rps-group-plc/fundamentals</t>
+  </si>
+  <si>
     <t>Costain Group</t>
   </si>
   <si>
+    <t>https://www.londonstockexchange.com/stock/COST/costain-group-plc/fundamentals</t>
+  </si>
+  <si>
     <t>Halma</t>
-  </si>
-  <si>
-    <t>https://www.londonstockexchange.com/stock/AFS/amiad-water-systems-ltd/fundamentals</t>
-  </si>
-  <si>
-    <t>https://www.londonstockexchange.com/stock/WATR/water-intelligence-plc/fundamentals</t>
-  </si>
-  <si>
-    <t>https://www.londonstockexchange.com/stock/RPS/rps-group-plc/fundamentals</t>
-  </si>
-  <si>
-    <t>https://www.londonstockexchange.com/stock/COST/costain-group-plc/fundamentals</t>
   </si>
   <si>
     <t>https://www.londonstockexchange.com/stock/HLMA/halma-plc/fundamentals</t>
@@ -75,7 +75,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -87,14 +87,6 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -117,18 +109,15 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -444,7 +433,7 @@
   <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -465,8 +454,8 @@
       <c r="A2" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="3" t="s">
-        <v>7</v>
+      <c r="B2" s="1" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -474,38 +463,35 @@
         <v>3</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="B4" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="B5" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="B6" t="s">
         <v>11</v>
       </c>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1" xr:uid="{1DDAEBEF-9BA3-4D8B-A843-5ABE568F6E36}"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId2"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>